<commit_message>
Mykyta fixed the bug!
</commit_message>
<xml_diff>
--- a/Dietary Guidelines.xlsx
+++ b/Dietary Guidelines.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Documents\MEGAsync\Zachary\Self\Programs\Python\NutritionResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEEAFC1-D4D1-4EFE-8176-3F7715FDF371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54234D11-99D6-4F5F-98A1-BB72DA883BA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="8640" windowHeight="4620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{31765216-1884-466A-A4C1-2332ACEA74B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dietary Guidelines" sheetId="1" r:id="rId1"/>
+    <sheet name="Dietary Guidelines 2015" sheetId="1" r:id="rId1"/>
+    <sheet name="Dietary Guidelines 2020" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="105">
   <si>
     <t>Macronutrients</t>
   </si>
@@ -218,6 +230,123 @@
   </si>
   <si>
     <t>10-35</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Calorie Level Assessed</t>
+  </si>
+  <si>
+    <t>Source of Goala</t>
+  </si>
+  <si>
+    <t>Protein (% kcal)</t>
+  </si>
+  <si>
+    <t>Protein (g)</t>
+  </si>
+  <si>
+    <t>Carbohydrate (% kcal)</t>
+  </si>
+  <si>
+    <t>Carbohydrate (g)</t>
+  </si>
+  <si>
+    <t>Fiber (g)</t>
+  </si>
+  <si>
+    <t>14g/ 1,000 kcal</t>
+  </si>
+  <si>
+    <t>Added Sugars (% kcal)</t>
+  </si>
+  <si>
+    <t>&lt;10</t>
+  </si>
+  <si>
+    <t>Total lipid (% kcal)</t>
+  </si>
+  <si>
+    <t>Saturated Fatty Acids (% kcal)</t>
+  </si>
+  <si>
+    <t>18:2 Linoleic acid (g)</t>
+  </si>
+  <si>
+    <t>18:3 Linoleic acid (g)</t>
+  </si>
+  <si>
+    <t>Calcium (mg)</t>
+  </si>
+  <si>
+    <t>1,000b</t>
+  </si>
+  <si>
+    <t>Iron (mg)</t>
+  </si>
+  <si>
+    <t>Magnesium (mg)</t>
+  </si>
+  <si>
+    <t>Phosphorus (mg)</t>
+  </si>
+  <si>
+    <t>Potassium (mg)</t>
+  </si>
+  <si>
+    <t>Sodium (mg)</t>
+  </si>
+  <si>
+    <t>CDRR</t>
+  </si>
+  <si>
+    <t>Zinc (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin A (mcg RAEd)</t>
+  </si>
+  <si>
+    <t>Vitamin E (mg ATd)</t>
+  </si>
+  <si>
+    <t>Vitamin D (IUd)</t>
+  </si>
+  <si>
+    <t>600c</t>
+  </si>
+  <si>
+    <t>Vitamin C (mg)</t>
+  </si>
+  <si>
+    <t>Thiamin (mg)</t>
+  </si>
+  <si>
+    <t>Riboflavin (mg)</t>
+  </si>
+  <si>
+    <t>Niacin (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B-6 (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin B-12 (mcg)</t>
+  </si>
+  <si>
+    <t>Choline (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin K (mcg)</t>
+  </si>
+  <si>
+    <t>Folate (mcg DFEd)</t>
+  </si>
+  <si>
+    <t>2-3</t>
   </si>
 </sst>
 </file>
@@ -707,10 +836,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1069,8 +1201,9 @@
   <dimension ref="A1:AJ16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2692,4 +2825,1730 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C45F8C-E997-4CEB-8B6D-0E616E3407D8}">
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+    </row>
+    <row r="2" spans="1:36" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="3">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3">
+        <v>130</v>
+      </c>
+      <c r="I4" s="3">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="3">
+        <v>7</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3">
+        <v>700</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>7</v>
+      </c>
+      <c r="R4" s="3">
+        <v>80</v>
+      </c>
+      <c r="S4" s="3">
+        <v>460</v>
+      </c>
+      <c r="T4" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1200</v>
+      </c>
+      <c r="V4" s="3">
+        <v>3</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3">
+        <v>300</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>15</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>6</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>200</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>30</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="3">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3">
+        <v>130</v>
+      </c>
+      <c r="I5" s="3">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" s="3">
+        <v>10</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>10</v>
+      </c>
+      <c r="R5" s="3">
+        <v>130</v>
+      </c>
+      <c r="S5" s="3">
+        <v>500</v>
+      </c>
+      <c r="T5" s="3">
+        <v>2300</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1500</v>
+      </c>
+      <c r="V5" s="3">
+        <v>5</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1200</v>
+      </c>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3">
+        <v>400</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>8</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>250</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>55</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1600</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="3">
+        <v>34</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3">
+        <v>130</v>
+      </c>
+      <c r="I6" s="3">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="3">
+        <v>10</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3">
+        <v>1300</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>8</v>
+      </c>
+      <c r="R6" s="3">
+        <v>240</v>
+      </c>
+      <c r="S6" s="3">
+        <v>1250</v>
+      </c>
+      <c r="T6" s="3">
+        <v>2300</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1800</v>
+      </c>
+      <c r="V6" s="3">
+        <v>8</v>
+      </c>
+      <c r="W6" s="3">
+        <v>1600</v>
+      </c>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3">
+        <v>600</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>45</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>12</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>375</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>60</v>
+      </c>
+      <c r="AJ6" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1800</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="3">
+        <v>46</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="3">
+        <v>130</v>
+      </c>
+      <c r="I7" s="3">
+        <v>25</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="3">
+        <v>11</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3">
+        <v>1300</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>15</v>
+      </c>
+      <c r="R7" s="3">
+        <v>360</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1250</v>
+      </c>
+      <c r="T7" s="3">
+        <v>2300</v>
+      </c>
+      <c r="U7" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V7" s="3">
+        <v>9</v>
+      </c>
+      <c r="W7" s="3">
+        <v>1800</v>
+      </c>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3">
+        <v>700</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>65</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>14</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>400</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>75</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="3">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="3">
+        <v>130</v>
+      </c>
+      <c r="I8" s="3">
+        <v>28</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="3">
+        <v>12</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>18</v>
+      </c>
+      <c r="R8" s="3">
+        <v>310</v>
+      </c>
+      <c r="S8" s="3">
+        <v>700</v>
+      </c>
+      <c r="T8" s="3">
+        <v>2600</v>
+      </c>
+      <c r="U8" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V8" s="3">
+        <v>8</v>
+      </c>
+      <c r="W8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3">
+        <v>700</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>75</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>14</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>425</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>90</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1800</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="3">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="3">
+        <v>130</v>
+      </c>
+      <c r="I9" s="3">
+        <v>25</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="3">
+        <v>12</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>18</v>
+      </c>
+      <c r="R9" s="3">
+        <v>320</v>
+      </c>
+      <c r="S9" s="3">
+        <v>700</v>
+      </c>
+      <c r="T9" s="3">
+        <v>2600</v>
+      </c>
+      <c r="U9" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V9" s="3">
+        <v>8</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1800</v>
+      </c>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3">
+        <v>700</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>75</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>425</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>90</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1600</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="3">
+        <v>46</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="3">
+        <v>130</v>
+      </c>
+      <c r="I10" s="3">
+        <v>22</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="3">
+        <v>11</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3">
+        <v>1200</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>8</v>
+      </c>
+      <c r="R10" s="3">
+        <v>320</v>
+      </c>
+      <c r="S10" s="3">
+        <v>700</v>
+      </c>
+      <c r="T10" s="3">
+        <v>2600</v>
+      </c>
+      <c r="U10" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V10" s="3">
+        <v>8</v>
+      </c>
+      <c r="W10" s="3">
+        <v>1600</v>
+      </c>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3">
+        <v>700</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>75</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>14</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>425</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>90</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="3">
+        <v>13</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="3">
+        <v>130</v>
+      </c>
+      <c r="I11" s="3">
+        <v>14</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="3">
+        <v>7</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3">
+        <v>700</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>7</v>
+      </c>
+      <c r="R11" s="3">
+        <v>80</v>
+      </c>
+      <c r="S11" s="3">
+        <v>460</v>
+      </c>
+      <c r="T11" s="3">
+        <v>2000</v>
+      </c>
+      <c r="U11" s="3">
+        <v>1200</v>
+      </c>
+      <c r="V11" s="3">
+        <v>3</v>
+      </c>
+      <c r="W11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3">
+        <v>300</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>15</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>200</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>30</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1400</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="3">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="3">
+        <v>130</v>
+      </c>
+      <c r="I12" s="3">
+        <v>20</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" s="3">
+        <v>10</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>10</v>
+      </c>
+      <c r="R12" s="3">
+        <v>130</v>
+      </c>
+      <c r="S12" s="3">
+        <v>500</v>
+      </c>
+      <c r="T12" s="3">
+        <v>2300</v>
+      </c>
+      <c r="U12" s="3">
+        <v>1500</v>
+      </c>
+      <c r="V12" s="3">
+        <v>5</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1400</v>
+      </c>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3">
+        <v>400</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>8</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>250</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>55</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1800</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="3">
+        <v>34</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="3">
+        <v>130</v>
+      </c>
+      <c r="I13" s="3">
+        <v>25</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" s="3">
+        <v>12</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3">
+        <v>1300</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>8</v>
+      </c>
+      <c r="R13" s="3">
+        <v>240</v>
+      </c>
+      <c r="S13" s="3">
+        <v>1250</v>
+      </c>
+      <c r="T13" s="3">
+        <v>2500</v>
+      </c>
+      <c r="U13" s="3">
+        <v>1800</v>
+      </c>
+      <c r="V13" s="3">
+        <v>8</v>
+      </c>
+      <c r="W13" s="3">
+        <v>1800</v>
+      </c>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3">
+        <v>600</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>45</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>12</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>375</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>60</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2200</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="3">
+        <v>52</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="3">
+        <v>130</v>
+      </c>
+      <c r="I14" s="3">
+        <v>31</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="3">
+        <v>16</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3">
+        <v>1300</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>11</v>
+      </c>
+      <c r="R14" s="3">
+        <v>410</v>
+      </c>
+      <c r="S14" s="3">
+        <v>1250</v>
+      </c>
+      <c r="T14" s="3">
+        <v>3000</v>
+      </c>
+      <c r="U14" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V14" s="3">
+        <v>11</v>
+      </c>
+      <c r="W14" s="3">
+        <v>2200</v>
+      </c>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3">
+        <v>900</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>75</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>16</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>550</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>75</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2400</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="3">
+        <v>56</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="3">
+        <v>130</v>
+      </c>
+      <c r="I15" s="3">
+        <v>34</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M15" s="3">
+        <v>17</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>8</v>
+      </c>
+      <c r="R15" s="3">
+        <v>400</v>
+      </c>
+      <c r="S15" s="3">
+        <v>700</v>
+      </c>
+      <c r="T15" s="3">
+        <v>3400</v>
+      </c>
+      <c r="U15" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V15" s="3">
+        <v>11</v>
+      </c>
+      <c r="W15" s="3">
+        <v>2400</v>
+      </c>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3">
+        <v>900</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>90</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>16</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>550</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>120</v>
+      </c>
+      <c r="AJ15" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2200</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="3">
+        <v>56</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="3">
+        <v>130</v>
+      </c>
+      <c r="I16" s="3">
+        <v>31</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M16" s="3">
+        <v>17</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>8</v>
+      </c>
+      <c r="R16" s="3">
+        <v>420</v>
+      </c>
+      <c r="S16" s="3">
+        <v>700</v>
+      </c>
+      <c r="T16" s="3">
+        <v>3400</v>
+      </c>
+      <c r="U16" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V16" s="3">
+        <v>11</v>
+      </c>
+      <c r="W16" s="3">
+        <v>2200</v>
+      </c>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3">
+        <v>900</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>600</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>90</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>16</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>550</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>120</v>
+      </c>
+      <c r="AJ16" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="3">
+        <v>56</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="3">
+        <v>130</v>
+      </c>
+      <c r="I17" s="3">
+        <v>28</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M17" s="3">
+        <v>14</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>8</v>
+      </c>
+      <c r="R17" s="3">
+        <v>420</v>
+      </c>
+      <c r="S17" s="3">
+        <v>700</v>
+      </c>
+      <c r="T17" s="3">
+        <v>3400</v>
+      </c>
+      <c r="U17" s="3">
+        <v>2300</v>
+      </c>
+      <c r="V17" s="3">
+        <v>11</v>
+      </c>
+      <c r="W17" s="3">
+        <v>2000</v>
+      </c>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3">
+        <v>900</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>90</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>16</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>550</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>120</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2020-'25 guidelines, guide_lookup() overhaul
</commit_message>
<xml_diff>
--- a/Dietary Guidelines.xlsx
+++ b/Dietary Guidelines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Documents\MEGAsync\Zachary\Self\Programs\Python\NutritionResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3486D702-318A-4091-9E7A-F287C12B9FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F27DAB-27CF-4E1C-89ED-C38ED0803F2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="6615" windowWidth="16230" windowHeight="15615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8040" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dietary Guidelines 2015" sheetId="1" r:id="rId1"/>
@@ -1199,7 +1199,7 @@
   <dimension ref="A1:AJ16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,15 +2826,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C45F8C-E997-4CEB-8B6D-0E616E3407D8}">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="18.28515625" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -4507,6 +4509,21 @@
         <v>400</v>
       </c>
     </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>